<commit_message>
Branch & Price: 1e RMP to be added
</commit_message>
<xml_diff>
--- a/Result/Result.xlsx
+++ b/Result/Result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emnormandie1-my.sharepoint.com/personal/jtang_em-normandie_fr/Documents/2EVRPMM/Result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1333" documentId="8_{92A22CC0-19AB-D84A-B77D-FA4F4CDBC343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5A12822-27F2-EE43-94F8-016FBF7C4E8B}"/>
+  <xr:revisionPtr revIDLastSave="1335" documentId="8_{92A22CC0-19AB-D84A-B77D-FA4F4CDBC343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FC07088-CEC3-46BE-B820-3F97E99B2146}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="6140" yWindow="500" windowWidth="28300" windowHeight="19860" activeTab="2" xr2:uid="{8802EF90-BEE6-8145-AE6F-1EA5C18B901E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8802EF90-BEE6-8145-AE6F-1EA5C18B901E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -639,18 +639,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -665,14 +665,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -680,7 +680,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1201,7 +1201,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1217,7 +1217,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1539,22 +1539,22 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.36328125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" customWidth="1"/>
+    <col min="6" max="6" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -1564,7 +1564,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1572,7 +1572,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4">
@@ -1588,7 +1588,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -1621,7 +1621,7 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="B7" s="1">
         <v>6</v>
       </c>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="B8" s="1">
         <v>8</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>849.53</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="3"/>
       <c r="B9" s="4">
         <v>10</v>
@@ -1669,67 +1669,67 @@
       </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -1745,38 +1745,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2688DEF4-29AA-4D4A-9F28-57B6F8D7E4AE}">
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" hidden="1" customWidth="1"/>
-    <col min="5" max="7" width="8.33203125" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="9.5" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" hidden="1" customWidth="1"/>
+    <col min="5" max="7" width="8.36328125" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="9.453125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.36328125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="5.453125" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="11" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="12.453125" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="18" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="10.1640625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="11.1640625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="3.83203125" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="15.36328125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1796875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="11.1796875" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="3.81640625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.453125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21">
       <c r="M2" t="s">
         <v>84</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21">
       <c r="A3" s="15"/>
       <c r="B3" s="16" t="s">
         <v>30</v>
@@ -1845,7 +1845,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21">
       <c r="A4" s="21" t="s">
         <v>32</v>
       </c>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="U4" s="24"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21">
       <c r="A5" s="77" t="s">
         <v>33</v>
       </c>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="U5" s="10"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21">
       <c r="A6" s="77" t="s">
         <v>34</v>
       </c>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="U6" s="10"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21">
       <c r="A7" s="77" t="s">
         <v>35</v>
       </c>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="U7" s="10"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21">
       <c r="A8" s="78" t="s">
         <v>36</v>
       </c>
@@ -2100,7 +2100,7 @@
       </c>
       <c r="U8" s="12"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21">
       <c r="A9" s="77" t="s">
         <v>37</v>
       </c>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="U9" s="24"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21">
       <c r="A10" s="77" t="s">
         <v>38</v>
       </c>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="U10" s="10"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21">
       <c r="A11" s="13" t="s">
         <v>39</v>
       </c>
@@ -2246,7 +2246,7 @@
       <c r="T11" s="72"/>
       <c r="U11" s="10"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21">
       <c r="A12" s="77" t="s">
         <v>40</v>
       </c>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="U12" s="10"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21">
       <c r="A13" s="13" t="s">
         <v>41</v>
       </c>
@@ -2344,7 +2344,7 @@
       <c r="T13" s="73"/>
       <c r="U13" s="12"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21">
       <c r="A14" s="55" t="s">
         <v>56</v>
       </c>
@@ -2395,7 +2395,7 @@
       </c>
       <c r="U14" s="24"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21">
       <c r="A15" s="61" t="s">
         <v>57</v>
       </c>
@@ -2446,7 +2446,7 @@
       </c>
       <c r="U15" s="10"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21">
       <c r="A16" s="61" t="s">
         <v>58</v>
       </c>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="U16" s="10"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21">
       <c r="A17" s="61" t="s">
         <v>59</v>
       </c>
@@ -2548,7 +2548,7 @@
       </c>
       <c r="U17" s="10"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21">
       <c r="A18" s="65" t="s">
         <v>60</v>
       </c>
@@ -2599,7 +2599,7 @@
       </c>
       <c r="U18" s="12"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21">
       <c r="A19" s="21" t="s">
         <v>62</v>
       </c>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="U19" s="24"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21">
       <c r="A20" s="13" t="s">
         <v>63</v>
       </c>
@@ -2709,7 +2709,7 @@
       </c>
       <c r="U20" s="10"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21">
       <c r="A21" s="13" t="s">
         <v>64</v>
       </c>
@@ -2764,7 +2764,7 @@
       </c>
       <c r="U21" s="10"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21">
       <c r="A22" s="13" t="s">
         <v>65</v>
       </c>
@@ -2819,7 +2819,7 @@
       </c>
       <c r="U22" s="10"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21">
       <c r="A23" s="14" t="s">
         <v>66</v>
       </c>
@@ -2874,7 +2874,7 @@
       </c>
       <c r="U23" s="12"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21">
       <c r="A24" s="13" t="s">
         <v>67</v>
       </c>
@@ -2929,7 +2929,7 @@
       </c>
       <c r="U24" s="24"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21">
       <c r="A25" s="77" t="s">
         <v>68</v>
       </c>
@@ -2986,7 +2986,7 @@
       </c>
       <c r="U25" s="10"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21">
       <c r="A26" s="13" t="s">
         <v>69</v>
       </c>
@@ -3034,7 +3034,7 @@
       </c>
       <c r="U26" s="10"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21">
       <c r="A27" s="13" t="s">
         <v>70</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21">
       <c r="A28" s="13" t="s">
         <v>71</v>
       </c>
@@ -3148,7 +3148,7 @@
       </c>
       <c r="U28" s="12"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21">
       <c r="A29" s="55" t="s">
         <v>72</v>
       </c>
@@ -3199,7 +3199,7 @@
       </c>
       <c r="U29" s="24"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21">
       <c r="A30" s="61" t="s">
         <v>73</v>
       </c>
@@ -3250,7 +3250,7 @@
       </c>
       <c r="U30" s="10"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21">
       <c r="A31" s="61" t="s">
         <v>74</v>
       </c>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="U31" s="10"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21">
       <c r="A32" s="61" t="s">
         <v>75</v>
       </c>
@@ -3352,7 +3352,7 @@
       </c>
       <c r="U32" s="10"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21">
       <c r="A33" s="65" t="s">
         <v>76</v>
       </c>
@@ -3413,33 +3413,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65939448-4F77-844B-8017-8175FCE85EC9}">
   <dimension ref="A1:BL42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView topLeftCell="A12" zoomScale="86" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" customWidth="1"/>
-    <col min="8" max="9" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.36328125" customWidth="1"/>
+    <col min="8" max="9" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.453125" bestFit="1" customWidth="1"/>
     <col min="12" max="16" width="11" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:64">
       <c r="A1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:64">
       <c r="A3" s="21"/>
       <c r="B3" s="30" t="s">
         <v>30</v>
@@ -3486,7 +3486,7 @@
       </c>
       <c r="S3" s="26"/>
     </row>
-    <row r="4" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:64" s="37" customFormat="1">
       <c r="A4" s="34" t="s">
         <v>32</v>
       </c>
@@ -3592,7 +3592,7 @@
       <c r="BK4"/>
       <c r="BL4"/>
     </row>
-    <row r="5" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:64" s="37" customFormat="1">
       <c r="A5" s="40" t="s">
         <v>32</v>
       </c>
@@ -3698,7 +3698,7 @@
       <c r="BK5"/>
       <c r="BL5"/>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:64">
       <c r="A6" s="9" t="s">
         <v>32</v>
       </c>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="S6" s="10"/>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:64">
       <c r="A7" s="9" t="s">
         <v>32</v>
       </c>
@@ -3820,7 +3820,7 @@
       </c>
       <c r="S7" s="10"/>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:64">
       <c r="A8" s="9" t="s">
         <v>32</v>
       </c>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="S8" s="10"/>
     </row>
-    <row r="9" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:64" s="37" customFormat="1">
       <c r="A9" s="40" t="s">
         <v>32</v>
       </c>
@@ -3987,7 +3987,7 @@
       <c r="BK9"/>
       <c r="BL9"/>
     </row>
-    <row r="10" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:64" s="37" customFormat="1">
       <c r="A10" s="34" t="s">
         <v>32</v>
       </c>
@@ -4093,7 +4093,7 @@
       <c r="BK10"/>
       <c r="BL10"/>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:64">
       <c r="A11" s="9" t="s">
         <v>32</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:64">
       <c r="A12" s="9" t="s">
         <v>32</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:64">
       <c r="A13" s="9" t="s">
         <v>32</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:64" s="37" customFormat="1">
       <c r="A14" s="40" t="s">
         <v>32</v>
       </c>
@@ -4388,7 +4388,7 @@
       <c r="BK14"/>
       <c r="BL14"/>
     </row>
-    <row r="15" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:64" s="37" customFormat="1">
       <c r="A15" s="40" t="s">
         <v>32</v>
       </c>
@@ -4494,7 +4494,7 @@
       <c r="BK15"/>
       <c r="BL15"/>
     </row>
-    <row r="16" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:64" s="37" customFormat="1">
       <c r="A16" s="34" t="s">
         <v>32</v>
       </c>
@@ -4600,7 +4600,7 @@
       <c r="BK16"/>
       <c r="BL16"/>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:64">
       <c r="A17" s="9" t="s">
         <v>32</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:64">
       <c r="A18" s="9" t="s">
         <v>32</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:64" s="37" customFormat="1">
       <c r="A19" s="40" t="s">
         <v>32</v>
       </c>
@@ -4832,7 +4832,7 @@
       <c r="BK19"/>
       <c r="BL19"/>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:64">
       <c r="A20" s="9" t="s">
         <v>32</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:64" s="37" customFormat="1">
       <c r="A21" s="47" t="s">
         <v>32</v>
       </c>
@@ -5001,7 +5001,7 @@
       <c r="BK21"/>
       <c r="BL21"/>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:64">
       <c r="A22" s="25" t="s">
         <v>32</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:64">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:64">
       <c r="A24" s="9" t="s">
         <v>32</v>
       </c>
@@ -5190,7 +5190,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:64">
       <c r="A25" s="9" t="s">
         <v>32</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:64" s="37" customFormat="1">
       <c r="A26" s="40" t="s">
         <v>32</v>
       </c>
@@ -5359,7 +5359,7 @@
       <c r="BK26"/>
       <c r="BL26"/>
     </row>
-    <row r="27" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:64" s="37" customFormat="1">
       <c r="A27" s="47" t="s">
         <v>32</v>
       </c>
@@ -5465,7 +5465,7 @@
       <c r="BK27"/>
       <c r="BL27"/>
     </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:64">
       <c r="A28" s="25" t="s">
         <v>32</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:64">
       <c r="A29" s="9" t="s">
         <v>32</v>
       </c>
@@ -5589,7 +5589,7 @@
       </c>
       <c r="S29" s="10"/>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:64">
       <c r="A30" s="9" t="s">
         <v>32</v>
       </c>
@@ -5655,7 +5655,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:64">
       <c r="A31" s="9" t="s">
         <v>32</v>
       </c>
@@ -5716,7 +5716,7 @@
       </c>
       <c r="S31" s="10"/>
     </row>
-    <row r="32" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:64" s="37" customFormat="1">
       <c r="A32" s="47" t="s">
         <v>32</v>
       </c>
@@ -5822,7 +5822,7 @@
       <c r="BK32"/>
       <c r="BL32"/>
     </row>
-    <row r="33" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:64">
       <c r="A33" s="25" t="s">
         <v>32</v>
       </c>
@@ -5883,7 +5883,7 @@
       </c>
       <c r="S33" s="24"/>
     </row>
-    <row r="34" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:64">
       <c r="A34" s="9" t="s">
         <v>32</v>
       </c>
@@ -5946,7 +5946,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:64" s="37" customFormat="1">
       <c r="A35" s="40" t="s">
         <v>32</v>
       </c>
@@ -6052,7 +6052,7 @@
       <c r="BK35"/>
       <c r="BL35"/>
     </row>
-    <row r="36" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:64">
       <c r="A36" s="11" t="s">
         <v>32</v>
       </c>
@@ -6115,7 +6115,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:64">
       <c r="A37" s="9" t="s">
         <v>32</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:64">
       <c r="A38" s="9" t="s">
         <v>32</v>
       </c>
@@ -6239,7 +6239,7 @@
       </c>
       <c r="S38" s="10"/>
     </row>
-    <row r="39" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:64" s="37" customFormat="1">
       <c r="A39" s="47" t="s">
         <v>32</v>
       </c>
@@ -6345,7 +6345,7 @@
       <c r="BK39"/>
       <c r="BL39"/>
     </row>
-    <row r="40" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:64">
       <c r="A40" s="9" t="s">
         <v>32</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:64" s="37" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:64" s="37" customFormat="1">
       <c r="A41" s="47" t="s">
         <v>32</v>
       </c>
@@ -6516,7 +6516,7 @@
       <c r="BK41"/>
       <c r="BL41"/>
     </row>
-    <row r="42" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:64">
       <c r="A42" s="11" t="s">
         <v>32</v>
       </c>
@@ -6587,19 +6587,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8198311A-D25E-EA42-9BFC-4E8254A78F38}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView zoomScale="108" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="108" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6328125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20">
       <c r="A1" s="79" t="s">
         <v>44</v>
       </c>
@@ -6623,7 +6623,7 @@
       <c r="S1" s="79"/>
       <c r="T1" s="79"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20">
       <c r="A2" s="79"/>
       <c r="B2" s="79"/>
       <c r="C2" s="79"/>
@@ -6645,7 +6645,7 @@
       <c r="S2" s="79"/>
       <c r="T2" s="79"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20">
       <c r="A3" s="80"/>
       <c r="B3" s="81" t="s">
         <v>50</v>
@@ -6678,7 +6678,7 @@
       <c r="S3" s="79"/>
       <c r="T3" s="79"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20">
       <c r="A4" s="83" t="s">
         <v>32</v>
       </c>
@@ -6720,7 +6720,7 @@
       <c r="S4" s="79"/>
       <c r="T4" s="79"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20">
       <c r="A5" s="84" t="s">
         <v>32</v>
       </c>
@@ -6762,7 +6762,7 @@
       <c r="S5" s="79"/>
       <c r="T5" s="79"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20">
       <c r="A6" s="84" t="s">
         <v>32</v>
       </c>
@@ -6804,7 +6804,7 @@
       <c r="S6" s="79"/>
       <c r="T6" s="79"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20">
       <c r="A7" s="84" t="s">
         <v>32</v>
       </c>
@@ -6846,7 +6846,7 @@
       <c r="S7" s="79"/>
       <c r="T7" s="79"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20">
       <c r="A8" s="84" t="s">
         <v>32</v>
       </c>
@@ -6888,7 +6888,7 @@
       <c r="S8" s="79"/>
       <c r="T8" s="79"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20">
       <c r="A9" s="84" t="s">
         <v>32</v>
       </c>
@@ -6928,7 +6928,7 @@
       <c r="S9" s="79"/>
       <c r="T9" s="79"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20">
       <c r="A10" s="83" t="s">
         <v>32</v>
       </c>
@@ -6970,7 +6970,7 @@
       <c r="S10" s="79"/>
       <c r="T10" s="79"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20">
       <c r="A11" s="84" t="s">
         <v>32</v>
       </c>
@@ -7012,7 +7012,7 @@
       <c r="S11" s="79"/>
       <c r="T11" s="79"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20">
       <c r="A12" s="84" t="s">
         <v>32</v>
       </c>
@@ -7054,7 +7054,7 @@
       <c r="S12" s="79"/>
       <c r="T12" s="79"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20">
       <c r="A13" s="84" t="s">
         <v>32</v>
       </c>
@@ -7088,7 +7088,7 @@
       <c r="S13" s="79"/>
       <c r="T13" s="79"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20">
       <c r="A14" s="84" t="s">
         <v>32</v>
       </c>
@@ -7122,7 +7122,7 @@
       <c r="S14" s="79"/>
       <c r="T14" s="79"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20">
       <c r="A15" s="84" t="s">
         <v>32</v>
       </c>
@@ -7163,7 +7163,7 @@
       <c r="S15" s="79"/>
       <c r="T15" s="79"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20">
       <c r="A16" s="83" t="s">
         <v>32</v>
       </c>
@@ -7203,7 +7203,7 @@
       <c r="S16" s="79"/>
       <c r="T16" s="79"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20">
       <c r="A17" s="84" t="s">
         <v>32</v>
       </c>
@@ -7244,7 +7244,7 @@
       <c r="S17" s="79"/>
       <c r="T17" s="79"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20">
       <c r="A18" s="84" t="s">
         <v>32</v>
       </c>
@@ -7285,7 +7285,7 @@
       <c r="S18" s="79"/>
       <c r="T18" s="79"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20">
       <c r="A19" s="84" t="s">
         <v>32</v>
       </c>
@@ -7327,7 +7327,7 @@
       <c r="S19" s="79"/>
       <c r="T19" s="79"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20">
       <c r="A20" s="84" t="s">
         <v>32</v>
       </c>
@@ -7369,7 +7369,7 @@
       <c r="S20" s="79"/>
       <c r="T20" s="79"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20">
       <c r="A21" s="87" t="s">
         <v>32</v>
       </c>
@@ -7411,7 +7411,7 @@
       <c r="S21" s="79"/>
       <c r="T21" s="79"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20">
       <c r="A22" s="84" t="s">
         <v>32</v>
       </c>
@@ -7453,7 +7453,7 @@
       <c r="S22" s="79"/>
       <c r="T22" s="79"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20">
       <c r="A23" s="84" t="s">
         <v>32</v>
       </c>
@@ -7495,7 +7495,7 @@
       <c r="S23" s="79"/>
       <c r="T23" s="79"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20">
       <c r="A24" s="84" t="s">
         <v>32</v>
       </c>
@@ -7537,7 +7537,7 @@
       <c r="S24" s="79"/>
       <c r="T24" s="79"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20">
       <c r="A25" s="84" t="s">
         <v>32</v>
       </c>
@@ -7579,7 +7579,7 @@
       <c r="S25" s="79"/>
       <c r="T25" s="79"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20">
       <c r="A26" s="84" t="s">
         <v>32</v>
       </c>
@@ -7621,7 +7621,7 @@
       <c r="S26" s="79"/>
       <c r="T26" s="79"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20">
       <c r="A27" s="87" t="s">
         <v>32</v>
       </c>
@@ -7663,7 +7663,7 @@
       <c r="S27" s="79"/>
       <c r="T27" s="79"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20">
       <c r="A28" s="84" t="s">
         <v>32</v>
       </c>
@@ -7705,7 +7705,7 @@
       <c r="S28" s="79"/>
       <c r="T28" s="79"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20">
       <c r="A29" s="84" t="s">
         <v>32</v>
       </c>
@@ -7747,7 +7747,7 @@
       <c r="S29" s="79"/>
       <c r="T29" s="79"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20">
       <c r="A30" s="84" t="s">
         <v>32</v>
       </c>
@@ -7789,7 +7789,7 @@
       <c r="S30" s="79"/>
       <c r="T30" s="79"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20">
       <c r="A31" s="84" t="s">
         <v>32</v>
       </c>
@@ -7831,7 +7831,7 @@
       <c r="S31" s="79"/>
       <c r="T31" s="79"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20">
       <c r="A32" s="87" t="s">
         <v>32</v>
       </c>
@@ -7873,7 +7873,7 @@
       <c r="S32" s="79"/>
       <c r="T32" s="79"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20">
       <c r="A33" s="84" t="s">
         <v>32</v>
       </c>
@@ -7915,7 +7915,7 @@
       <c r="S33" s="79"/>
       <c r="T33" s="79"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20">
       <c r="A34" s="84" t="s">
         <v>32</v>
       </c>
@@ -7957,7 +7957,7 @@
       <c r="S34" s="79"/>
       <c r="T34" s="79"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20">
       <c r="A35" s="84" t="s">
         <v>32</v>
       </c>
@@ -7999,7 +7999,7 @@
       <c r="S35" s="79"/>
       <c r="T35" s="79"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20">
       <c r="A36" s="87" t="s">
         <v>32</v>
       </c>
@@ -8041,7 +8041,7 @@
       <c r="S36" s="79"/>
       <c r="T36" s="79"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20">
       <c r="A37" s="84" t="s">
         <v>32</v>
       </c>
@@ -8083,7 +8083,7 @@
       <c r="S37" s="79"/>
       <c r="T37" s="79"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20">
       <c r="A38" s="84" t="s">
         <v>32</v>
       </c>
@@ -8125,7 +8125,7 @@
       <c r="S38" s="79"/>
       <c r="T38" s="79"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20">
       <c r="A39" s="87" t="s">
         <v>32</v>
       </c>
@@ -8167,7 +8167,7 @@
       <c r="S39" s="79"/>
       <c r="T39" s="79"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20">
       <c r="A40" s="84" t="s">
         <v>32</v>
       </c>
@@ -8209,7 +8209,7 @@
       <c r="S40" s="79"/>
       <c r="T40" s="79"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20">
       <c r="A41" s="87" t="s">
         <v>32</v>
       </c>
@@ -8251,7 +8251,7 @@
       <c r="S41" s="79"/>
       <c r="T41" s="79"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20">
       <c r="A42" s="87" t="s">
         <v>32</v>
       </c>

</xml_diff>